<commit_message>
Initial commit I guess, a little late!
</commit_message>
<xml_diff>
--- a/PredictedAges.xlsx
+++ b/PredictedAges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\Graduate School\Summer 2019\Chen Research\BrainAgePredictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63239D09-5DCA-4A78-9DBB-79035927B20E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD62A4E-D6DF-495C-B009-D936FF2DB14E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7785" xr2:uid="{3ABF37D0-9CE1-4972-898F-CECF5263D171}"/>
   </bookViews>
@@ -685,11 +685,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,112 +816,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>1.84481388919844</c:v>
+                  <c:v>-13.601594582351099</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.214365503752799</c:v>
+                  <c:v>10.6665566133375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.941196431088901</c:v>
+                  <c:v>-8.6821511934090198E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.0618842114425</c:v>
+                  <c:v>-0.64267623116005201</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.869056664677899</c:v>
+                  <c:v>11.3602594163678</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.34038770701646798</c:v>
+                  <c:v>12.123667049830299</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.5137995561728204</c:v>
+                  <c:v>18.671589562352601</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.64747957244321697</c:v>
+                  <c:v>-5.2145677958866798</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.2393016077921901</c:v>
+                  <c:v>7.0165939416493703</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.51454080130173396</c:v>
+                  <c:v>3.96567983792389</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.76478835539725698</c:v>
+                  <c:v>2.6429811818782798</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.187426527661813</c:v>
+                  <c:v>7.7929654887514301</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.8867108848863</c:v>
+                  <c:v>-19.526122135978</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.7404410174261704</c:v>
+                  <c:v>4.1608377028338799</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.8220371186592</c:v>
+                  <c:v>8.4526280968683203</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.27127002302890402</c:v>
+                  <c:v>-0.475036619129731</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.2245173855012297</c:v>
+                  <c:v>-5.5415302566624902</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.9962941129503</c:v>
+                  <c:v>-0.66792906667808405</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.5204405861552299</c:v>
+                  <c:v>-5.7968973045812797</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.6031929917803098</c:v>
+                  <c:v>-15.637360519805201</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.4259324710846597</c:v>
+                  <c:v>-11.805903242207799</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.23709501436291</c:v>
+                  <c:v>0.51650861183276198</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6.8138756067285797</c:v>
+                  <c:v>-1.99019756474065</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.8939750975974503</c:v>
+                  <c:v>9.3005934962305101</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6.4953294362230496</c:v>
+                  <c:v>-9.1124708189614196</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.19830487050766199</c:v>
+                  <c:v>1.5585622901790399</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>11.8662147089616</c:v>
+                  <c:v>-6.3394826997406897</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8.8661965746576499</c:v>
+                  <c:v>-7.6464748701648704</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>16.450615840624</c:v>
+                  <c:v>-7.7996936103173198</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.8449766131376801</c:v>
+                  <c:v>-0.162984122908468</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>21.180681066088599</c:v>
+                  <c:v>5.0825203412631401</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.8737929969041005</c:v>
+                  <c:v>-9.7266780688147794</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.9965698473669198</c:v>
+                  <c:v>-16.0812623813603</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7.0846291386143596</c:v>
+                  <c:v>-8.4565492026295797</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>9.0760237921857208</c:v>
+                  <c:v>-4.2859005183277601</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.1595080661952499</c:v>
+                  <c:v>-3.8084956051466099</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1008,6 +1009,8 @@
         <c:axId val="617942848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="40"/>
+          <c:min val="-40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1225,124 +1228,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>6.3286366716108802</c:v>
+                  <c:v>-3.19735007500512</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.680223755055501</c:v>
+                  <c:v>-9.1394860962673405</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.538117064967899</c:v>
+                  <c:v>-15.530545268379999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.33464270373703098</c:v>
+                  <c:v>-6.7535455027815701</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1904231097021798</c:v>
+                  <c:v>-5.1548403660301698</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.7353881123697406</c:v>
+                  <c:v>6.3241103629234203</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27.1440037676347</c:v>
+                  <c:v>20.980672737769101</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.899923254606099</c:v>
+                  <c:v>12.497745795365899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.6365659128640404</c:v>
+                  <c:v>4.6524424744500896</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.507955970727899</c:v>
+                  <c:v>-8.8081493932750092</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.9108479109046597</c:v>
+                  <c:v>-2.7262205150035901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.3612623955480201</c:v>
+                  <c:v>-4.6725290353381501</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.880088939413801</c:v>
+                  <c:v>6.0321506036901598</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.9144541643394799</c:v>
+                  <c:v>4.2715304554659701</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.4693806153870899</c:v>
+                  <c:v>-5.8422364342808102</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.65464752602135601</c:v>
+                  <c:v>-4.3221392613941703</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.3019010713872201</c:v>
+                  <c:v>-2.14302454937557</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.944921697760799</c:v>
+                  <c:v>0.75108225712577303</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17.694787007852199</c:v>
+                  <c:v>-5.2488171019544003</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.6065600338479902</c:v>
+                  <c:v>9.4845437890954098</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.77542275929788196</c:v>
+                  <c:v>-1.5508923518167499</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>22.830946024283499</c:v>
+                  <c:v>0.65629795511721001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11.717727235283901</c:v>
+                  <c:v>2.3453819865366898</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.2007215871474095</c:v>
+                  <c:v>22.0147250807943</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.4962078606849296</c:v>
+                  <c:v>14.463907616954399</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>22.897312463648099</c:v>
+                  <c:v>-15.3331570918397</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8.4855965560022</c:v>
+                  <c:v>6.8391448391957796</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.58530590520489001</c:v>
+                  <c:v>-7.0569841875738604</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10.493875897957301</c:v>
+                  <c:v>2.6272591521403599</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>18.7666491035415</c:v>
+                  <c:v>-6.5425641135263604</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5.56321196868159</c:v>
+                  <c:v>-3.4432108122736298</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>12.632758538814</c:v>
+                  <c:v>-9.2317269500347603</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>7.6735490383337401</c:v>
+                  <c:v>1.5429043739241699</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.1556696677537999</c:v>
+                  <c:v>-2.8012019126312402</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.116849269438212</c:v>
+                  <c:v>1.64183214359008</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.41847534770148</c:v>
+                  <c:v>0.32359814196172398</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>10.266870205308701</c:v>
+                  <c:v>10.320866247558101</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>12.997018417301399</c:v>
+                  <c:v>-10.073056296894199</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.30804573546692599</c:v>
+                  <c:v>2.4539090046405301</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.51351604805616802</c:v>
+                  <c:v>15.238080680115999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1430,6 +1433,8 @@
         <c:axId val="806207848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="40"/>
+          <c:min val="-40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1616,10 +1621,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.0469816272965886E-2"/>
-          <c:y val="2.5428331875182269E-2"/>
+          <c:x val="6.3485341108477839E-2"/>
+          <c:y val="0.16772603924051915"/>
           <c:w val="0.89019685039370078"/>
-          <c:h val="0.72088764946048411"/>
+          <c:h val="0.78056096506636707"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1657,232 +1662,232 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>10.208142259738301</c:v>
+                  <c:v>14.3886019441857</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.509344858196499</c:v>
+                  <c:v>20.510397518750199</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.639628033649799</c:v>
+                  <c:v>-14.1374501748348</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.592823587365499</c:v>
+                  <c:v>-17.436508794311301</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.100175733311907</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.9151124965787902</c:v>
+                  <c:v>0.63166691686765097</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>8.1491968252612708</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.10006431567207801</c:v>
+                  <c:v>6.5414823802906996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.8684630194206999</c:v>
+                  <c:v>-8.0498700992472703</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.2134867614014699</c:v>
+                  <c:v>5.9238511549052797</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.7248266065115203</c:v>
+                  <c:v>8.6846288439479196</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.10021531347167199</c:v>
+                  <c:v>-3.98896539106555</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.1653191916769599</c:v>
+                  <c:v>12.2304511401134</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.0665945746353298</c:v>
+                  <c:v>2.4724052142890001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.5466848451715904</c:v>
+                  <c:v>15.887867626020199</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13.414587477303099</c:v>
+                  <c:v>9.2187482662492606</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18.384294957962101</c:v>
+                  <c:v>2.2753854943249698</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.53057455596572101</c:v>
+                  <c:v>13.2708472686727</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16.725690186318001</c:v>
+                  <c:v>-7.0136259576629003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.3072671157031799</c:v>
+                  <c:v>-3.4713442820627098</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.3804449523492801</c:v>
+                  <c:v>-12.1724464665381</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.4072652906522602</c:v>
+                  <c:v>6.8126554230456504</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10.649336197693</c:v>
+                  <c:v>8.8778949821816902</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.4161615820236397</c:v>
+                  <c:v>6.8402086108286202</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.2320409343899899</c:v>
+                  <c:v>5.6996856165220304</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.8739564460459901</c:v>
+                  <c:v>-6.7824008880150597</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.2556245513178697</c:v>
+                  <c:v>-0.86321123485502904</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9.7502588331067699</c:v>
+                  <c:v>3.1388175106930398</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.6231599769743901</c:v>
+                  <c:v>-15.025150968262899</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>12.390059839360299</c:v>
+                  <c:v>-2.3874083016165102</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9.9888625995127697E-2</c:v>
+                  <c:v>6.7139042627097396</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>10.310072426543901</c:v>
+                  <c:v>1.4916554308821599</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.6186453836000902</c:v>
+                  <c:v>5.3216613662554098</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.6737603776290495</c:v>
+                  <c:v>11.8772056038489</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.3583558769450801</c:v>
+                  <c:v>-2.4933496765415399</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.83639790018132</c:v>
+                  <c:v>-3.3280991437122598</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.96855244665155704</c:v>
+                  <c:v>-4.8121261406532696</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>9.7366651947491896</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>5.9949169068360098</c:v>
+                  <c:v>-2.5775435070594699</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0.00E+00">
+                  <c:v>4.99620745771358</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.100378316907402</c:v>
+                  <c:v>-2.5373296176344602</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>16.3766077001236</c:v>
+                  <c:v>-12.162549817272501</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>9.4559633538376602</c:v>
+                  <c:v>-5.8590324797576798</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.69976367579258</c:v>
+                  <c:v>-2.61294454765327</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>9.9936584750466295E-2</c:v>
+                  <c:v>2.19102254823179</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.6217504606270898</c:v>
+                  <c:v>13.4285633467907</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4.8413128779802701</c:v>
+                  <c:v>-1.79572549341105</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>12.2120700725178</c:v>
+                  <c:v>-15.1830059519081</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>7.10775015360786</c:v>
+                  <c:v>0.46321920883848799</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>11.3991058040725</c:v>
+                  <c:v>5.4073078213821404</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.77282755764241</c:v>
+                  <c:v>9.5648314155457896</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>13.2678584065925</c:v>
+                  <c:v>4.7501783104002504</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>5.0009354077862502</c:v>
+                  <c:v>1.8248496956710301</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>7.5348078488976498</c:v>
+                  <c:v>3.2090998231557899</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>3.3584938504079802</c:v>
+                  <c:v>-7.9257195972674701</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>8.4588180788019507</c:v>
+                  <c:v>-2.79533845356009</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>5.1784817260097702</c:v>
+                  <c:v>-4.4228831706254201</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>9.9863350681658802E-2</c:v>
+                  <c:v>3.65063598266009</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.8284513039649299</c:v>
+                  <c:v>3.8555922744845601</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.1448483542264398</c:v>
+                  <c:v>-3.6033895512207099</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>7.07148589689153</c:v>
+                  <c:v>-3.8137599526650798</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.100161355049785</c:v>
+                  <c:v>-12.330320590586</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.61533170054900599</c:v>
+                  <c:v>12.055740396794899</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.100283055795948</c:v>
+                  <c:v>0.40871853304422201</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>9.4827797483235905</c:v>
+                  <c:v>-9.7901364052635795</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>17.8787580990283</c:v>
+                  <c:v>-12.451641834077201</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.10001499934843799</c:v>
+                  <c:v>-2.16595890789318</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.10028298895356599</c:v>
+                  <c:v>-6.1072529117890504</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.4618938742061101</c:v>
+                  <c:v>-7.5415369459472501</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.100163878478056</c:v>
+                  <c:v>-6.4451178469617698</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5.3356933320842996</c:v>
+                  <c:v>-14.9190926712446</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.10017903007327</c:v>
+                  <c:v>15.2213573222023</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>6.96651525276814</c:v>
+                  <c:v>-4.28807914748554</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>6.0205347725268101</c:v>
+                  <c:v>-20.40001573488</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>9.9724611701986904E-2</c:v>
+                  <c:v>3.9214288238769299</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>9.3323620992515703</c:v>
+                  <c:v>-7.6730559976499899</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1.57084135308864</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.100484310038918</c:v>
+                  <c:v>5.0057380389832096</c:v>
+                </c:pt>
+                <c:pt idx="75" formatCode="0.00E+00">
+                  <c:v>4.4496782525720304</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1970,6 +1975,8 @@
         <c:axId val="804253552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="40"/>
+          <c:min val="-40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2192,139 +2199,139 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="0">
-                  <c:v>19.114611776724999</c:v>
+                  <c:v>30.7898971034334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9242158439568602</c:v>
+                  <c:v>-1.5771117437567901</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.0848513919514</c:v>
+                  <c:v>21.1055247956328</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.63293687866478</c:v>
+                  <c:v>1.1018096509234701</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.696595013154599</c:v>
+                  <c:v>24.137442188843998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.469352092826099</c:v>
+                  <c:v>14.378932588657801</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3761168544461599</c:v>
+                  <c:v>7.6832280872506598</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.186284558813298</c:v>
+                  <c:v>8.8172144904965801</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.0888283513966</c:v>
+                  <c:v>12.393331186656299</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.5484848570393197</c:v>
+                  <c:v>7.8408618956829903</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.8411563650452498</c:v>
+                  <c:v>11.043056252657999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.6976498786010099</c:v>
+                  <c:v>3.3449030721937598</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19.908904410342199</c:v>
+                  <c:v>22.106112259263099</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.73758893247531</c:v>
+                  <c:v>9.5057760020731603</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24.5494130172561</c:v>
+                  <c:v>12.8370447637579</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21.0076805339266</c:v>
+                  <c:v>-13.54910157129</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.1451369699428904</c:v>
+                  <c:v>-4.4695806199546997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.4534516837686997</c:v>
+                  <c:v>-6.79098535943454</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16.364936484010698</c:v>
+                  <c:v>16.937331736953102</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13.150335478263001</c:v>
+                  <c:v>17.597791262280499</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.677147574970277</c:v>
+                  <c:v>16.761978630563501</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10.9285282958314</c:v>
+                  <c:v>10.5016210600348</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11.6224628448481</c:v>
+                  <c:v>11.874015707950701</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10.826862104934699</c:v>
+                  <c:v>9.5627567651437992</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>13.362154745594401</c:v>
+                  <c:v>9.0630388889924092</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>13.711605167763</c:v>
+                  <c:v>7.1970293184230503</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.2497570321114599</c:v>
+                  <c:v>-8.23297899317601</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>16.072207189195701</c:v>
+                  <c:v>3.3666131337578098</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.39416207396519098</c:v>
+                  <c:v>-12.2751211142402</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>8.7201920350790996</c:v>
+                  <c:v>8.3295493090657899</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>21.609762225137899</c:v>
+                  <c:v>7.2737829316659797</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.40857966081365</c:v>
+                  <c:v>-0.25433353425597299</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>12.0077350373651</c:v>
+                  <c:v>13.3627470318796</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>17.956310265383902</c:v>
+                  <c:v>15.4100325708149</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>15.212780580663701</c:v>
+                  <c:v>11.0902206449829</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>7.1340462039309704</c:v>
+                  <c:v>-6.5676839552624298</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.4645287696572202</c:v>
+                  <c:v>-4.4127732573008904</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>7.1740363264026099</c:v>
+                  <c:v>9.2235310011821507</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>6.2248321261751904</c:v>
+                  <c:v>1.7296402357651499</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>10.3339541033138</c:v>
+                  <c:v>9.2792505667739604</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>10.745369701861501</c:v>
+                  <c:v>11.6444415207906</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>19.062548244156702</c:v>
+                  <c:v>-0.52900101693870705</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>14.0643443008054</c:v>
+                  <c:v>6.2340362137716596</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>17.914047741483099</c:v>
+                  <c:v>18.289430615348099</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>18.4517146955809</c:v>
+                  <c:v>29.9219942017492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2412,6 +2419,8 @@
         <c:axId val="812979192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="40"/>
+          <c:min val="-40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4750,16 +4759,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>448235</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>99172</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>147917</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>40341</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4789,15 +4798,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:colOff>434788</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>147918</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>129988</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>90768</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4865,15 +4874,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>147918</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>106456</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>448236</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>49306</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5202,8 +5211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AED9FECA-6B76-47AC-86F7-79CBFE132841}">
   <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5241,10 +5250,10 @@
         <v>19</v>
       </c>
       <c r="D2">
-        <v>29.208142259738299</v>
+        <v>32.119639435593399</v>
       </c>
       <c r="E2">
-        <v>10.208142259738301</v>
+        <v>14.3886019441857</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5258,10 +5267,10 @@
         <v>20</v>
       </c>
       <c r="D3">
-        <v>40.509344858196499</v>
+        <v>30.769683390158502</v>
       </c>
       <c r="E3">
-        <v>20.509344858196499</v>
+        <v>20.510397518750199</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5275,10 +5284,10 @@
         <v>54</v>
       </c>
       <c r="D4">
-        <v>36.360371966350101</v>
+        <v>41.715387982893198</v>
       </c>
       <c r="E4">
-        <v>17.639628033649799</v>
+        <v>-14.1374501748348</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5292,10 +5301,10 @@
         <v>51</v>
       </c>
       <c r="D5">
-        <v>39.407176412634399</v>
+        <v>42.6469952119783</v>
       </c>
       <c r="E5">
-        <v>11.592823587365499</v>
+        <v>-17.436508794311301</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5309,10 +5318,10 @@
         <v>30</v>
       </c>
       <c r="D6">
-        <v>29.899824266688</v>
+        <v>23.3457938449186</v>
       </c>
       <c r="E6">
-        <v>0.100175733311907</v>
+        <v>0.63166691686765097</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5326,10 +5335,10 @@
         <v>25</v>
       </c>
       <c r="D7">
-        <v>30.915112496578701</v>
-      </c>
-      <c r="E7">
-        <v>5.9151124965787902</v>
+        <v>29.704655116804599</v>
+      </c>
+      <c r="E7" s="4">
+        <v>8.1491968252612708</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5343,10 +5352,10 @@
         <v>24</v>
       </c>
       <c r="D8">
-        <v>24.100064315672</v>
+        <v>28.9519966336354</v>
       </c>
       <c r="E8">
-        <v>0.10006431567207801</v>
+        <v>6.5414823802906996</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5360,10 +5369,10 @@
         <v>48</v>
       </c>
       <c r="D9">
-        <v>39.131536980579199</v>
+        <v>41.364803660859799</v>
       </c>
       <c r="E9">
-        <v>8.8684630194206999</v>
+        <v>-8.0498700992472703</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5377,10 +5386,10 @@
         <v>28</v>
       </c>
       <c r="D10">
-        <v>30.213486761401398</v>
+        <v>24.731970441198101</v>
       </c>
       <c r="E10">
-        <v>2.2134867614014699</v>
+        <v>5.9238511549052797</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5394,10 +5403,10 @@
         <v>29</v>
       </c>
       <c r="D11">
-        <v>33.724826606511499</v>
+        <v>37.703528669159802</v>
       </c>
       <c r="E11">
-        <v>4.7248266065115203</v>
+        <v>8.6846288439479196</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5411,10 +5420,10 @@
         <v>33</v>
       </c>
       <c r="D12">
-        <v>33.100215313471601</v>
+        <v>35.422496933982998</v>
       </c>
       <c r="E12">
-        <v>0.10021531347167199</v>
+        <v>-3.98896539106555</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5428,10 +5437,10 @@
         <v>25</v>
       </c>
       <c r="D13">
-        <v>30.1653191916769</v>
+        <v>24.8847404089788</v>
       </c>
       <c r="E13">
-        <v>5.1653191916769599</v>
+        <v>12.2304511401134</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5445,10 +5454,10 @@
         <v>27</v>
       </c>
       <c r="D14">
-        <v>20.933405425364601</v>
+        <v>24.0013642023663</v>
       </c>
       <c r="E14">
-        <v>6.0665945746353298</v>
+        <v>2.4724052142890001</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5462,10 +5471,10 @@
         <v>23</v>
       </c>
       <c r="D15">
-        <v>28.546684845171502</v>
+        <v>25.867897411403401</v>
       </c>
       <c r="E15">
-        <v>5.5466848451715904</v>
+        <v>15.887867626020199</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5479,10 +5488,10 @@
         <v>24</v>
       </c>
       <c r="D16">
-        <v>37.414587477303101</v>
+        <v>33.902300168597101</v>
       </c>
       <c r="E16">
-        <v>13.414587477303099</v>
+        <v>9.2187482662492606</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5496,10 +5505,10 @@
         <v>21</v>
       </c>
       <c r="D17">
-        <v>39.384294957962098</v>
+        <v>33.281995092667898</v>
       </c>
       <c r="E17">
-        <v>18.384294957962101</v>
+        <v>2.2753854943249698</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5513,10 +5522,10 @@
         <v>26</v>
       </c>
       <c r="D18">
-        <v>26.5305745559657</v>
+        <v>23.1183715922981</v>
       </c>
       <c r="E18">
-        <v>0.53057455596572101</v>
+        <v>13.2708472686727</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5530,10 +5539,10 @@
         <v>50</v>
       </c>
       <c r="D19">
-        <v>33.274309813681903</v>
+        <v>33.911535682018702</v>
       </c>
       <c r="E19">
-        <v>16.725690186318001</v>
+        <v>-7.0136259576629003</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5547,10 +5556,10 @@
         <v>57</v>
       </c>
       <c r="D20">
-        <v>54.692732884296802</v>
+        <v>60.255969598843201</v>
       </c>
       <c r="E20">
-        <v>2.3072671157031799</v>
+        <v>-3.4713442820627098</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5564,10 +5573,10 @@
         <v>46</v>
       </c>
       <c r="D21">
-        <v>44.619555047650699</v>
+        <v>45.712892526823502</v>
       </c>
       <c r="E21">
-        <v>1.3804449523492801</v>
+        <v>-12.1724464665381</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5581,10 +5590,10 @@
         <v>25</v>
       </c>
       <c r="D22">
-        <v>29.407265290652202</v>
+        <v>30.866876068241702</v>
       </c>
       <c r="E22">
-        <v>4.4072652906522602</v>
+        <v>6.8126554230456504</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5598,10 +5607,10 @@
         <v>24</v>
       </c>
       <c r="D23">
-        <v>34.649336197693003</v>
+        <v>32.810100695217102</v>
       </c>
       <c r="E23">
-        <v>10.649336197693</v>
+        <v>8.8778949821816902</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5615,10 +5624,10 @@
         <v>35</v>
       </c>
       <c r="D24">
-        <v>40.416161582023598</v>
+        <v>47.4860622691765</v>
       </c>
       <c r="E24">
-        <v>5.4161615820236397</v>
+        <v>6.8402086108286202</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5632,10 +5641,10 @@
         <v>29</v>
       </c>
       <c r="D25">
-        <v>33.2320409343899</v>
+        <v>38.144236735122298</v>
       </c>
       <c r="E25">
-        <v>4.2320409343899899</v>
+        <v>5.6996856165220304</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5649,10 +5658,10 @@
         <v>26</v>
       </c>
       <c r="D26">
-        <v>24.126043553953998</v>
+        <v>20.4722448817116</v>
       </c>
       <c r="E26">
-        <v>1.8739564460459901</v>
+        <v>-6.7824008880150597</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5666,10 +5675,10 @@
         <v>25</v>
       </c>
       <c r="D27">
-        <v>29.255624551317801</v>
+        <v>31.220234333317801</v>
       </c>
       <c r="E27">
-        <v>4.2556245513178697</v>
+        <v>-0.86321123485502904</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5683,10 +5692,10 @@
         <v>27</v>
       </c>
       <c r="D28">
-        <v>36.750258833106699</v>
+        <v>35.793553783062002</v>
       </c>
       <c r="E28">
-        <v>9.7502588331067699</v>
+        <v>3.1388175106930398</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5700,10 +5709,10 @@
         <v>58</v>
       </c>
       <c r="D29">
-        <v>59.623159976974399</v>
+        <v>61.294868173285103</v>
       </c>
       <c r="E29">
-        <v>1.6231599769743901</v>
+        <v>-15.025150968262899</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5717,10 +5726,10 @@
         <v>52</v>
       </c>
       <c r="D30">
-        <v>39.609940160639603</v>
+        <v>44.210909840159196</v>
       </c>
       <c r="E30">
-        <v>12.390059839360299</v>
+        <v>-2.3874083016165102</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5734,10 +5743,10 @@
         <v>24</v>
       </c>
       <c r="D31">
-        <v>24.099888625995099</v>
+        <v>19.206332637845499</v>
       </c>
       <c r="E31">
-        <v>9.9888625995127697E-2</v>
+        <v>6.7139042627097396</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5751,10 +5760,10 @@
         <v>23</v>
       </c>
       <c r="D32">
-        <v>33.310072426543897</v>
+        <v>26.5069499212076</v>
       </c>
       <c r="E32">
-        <v>10.310072426543901</v>
+        <v>1.4916554308821599</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5768,10 +5777,10 @@
         <v>28</v>
       </c>
       <c r="D33">
-        <v>32.618645383600096</v>
+        <v>34.196576658387301</v>
       </c>
       <c r="E33">
-        <v>4.6186453836000902</v>
+        <v>5.3216613662554098</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5785,10 +5794,10 @@
         <v>25</v>
       </c>
       <c r="D34">
-        <v>33.673760377629002</v>
+        <v>32.784062083122599</v>
       </c>
       <c r="E34">
-        <v>8.6737603776290495</v>
+        <v>11.8772056038489</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5802,10 +5811,10 @@
         <v>33</v>
       </c>
       <c r="D35">
-        <v>29.641644123054899</v>
+        <v>35.543091106347397</v>
       </c>
       <c r="E35">
-        <v>3.3583558769450801</v>
+        <v>-2.4933496765415399</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5819,10 +5828,10 @@
         <v>38</v>
       </c>
       <c r="D36">
-        <v>40.836397900181296</v>
+        <v>46.248031308723199</v>
       </c>
       <c r="E36">
-        <v>2.83639790018132</v>
+        <v>-3.3280991437122598</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5836,10 +5845,10 @@
         <v>46</v>
       </c>
       <c r="D37">
-        <v>45.0314475533484</v>
+        <v>41.861953159535901</v>
       </c>
       <c r="E37">
-        <v>0.96855244665155704</v>
+        <v>-4.8121261406532696</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5853,10 +5862,10 @@
         <v>43</v>
       </c>
       <c r="D38">
-        <v>33.2633348052508</v>
+        <v>35.723429237618198</v>
       </c>
       <c r="E38">
-        <v>9.7366651947491896</v>
+        <v>-2.5775435070594699</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5870,10 +5879,10 @@
         <v>32</v>
       </c>
       <c r="D39">
-        <v>37.994916906836004</v>
-      </c>
-      <c r="E39">
-        <v>5.9949169068360098</v>
+        <v>34.42460152444</v>
+      </c>
+      <c r="E39" s="4">
+        <v>4.99620745771358</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5887,10 +5896,10 @@
         <v>46</v>
       </c>
       <c r="D40">
-        <v>46.100378316907403</v>
+        <v>48.847653118657597</v>
       </c>
       <c r="E40">
-        <v>0.100378316907402</v>
+        <v>-2.5373296176344602</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5904,10 +5913,10 @@
         <v>53</v>
       </c>
       <c r="D41">
-        <v>36.623392299876301</v>
+        <v>44.674244490650899</v>
       </c>
       <c r="E41">
-        <v>16.3766077001236</v>
+        <v>-12.162549817272501</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5921,10 +5930,10 @@
         <v>50</v>
       </c>
       <c r="D42">
-        <v>40.544036646162297</v>
+        <v>39.4073212031523</v>
       </c>
       <c r="E42">
-        <v>9.4559633538376602</v>
+        <v>-5.8590324797576798</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5938,10 +5947,10 @@
         <v>54</v>
       </c>
       <c r="D43">
-        <v>49.300236324207397</v>
+        <v>53.857865340382197</v>
       </c>
       <c r="E43">
-        <v>4.69976367579258</v>
+        <v>-2.61294454765327</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5955,10 +5964,10 @@
         <v>51</v>
       </c>
       <c r="D44">
-        <v>50.900063415249498</v>
+        <v>50.362011123570603</v>
       </c>
       <c r="E44">
-        <v>9.9936584750466295E-2</v>
+        <v>2.19102254823179</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5972,10 +5981,10 @@
         <v>20</v>
       </c>
       <c r="D45">
-        <v>24.621750460626998</v>
+        <v>24.709288549230799</v>
       </c>
       <c r="E45">
-        <v>4.6217504606270898</v>
+        <v>13.4285633467907</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5989,10 +5998,10 @@
         <v>24</v>
       </c>
       <c r="D46">
-        <v>28.841312877980201</v>
+        <v>29.242293322823599</v>
       </c>
       <c r="E46">
-        <v>4.8413128779802701</v>
+        <v>-1.79572549341105</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6006,10 +6015,10 @@
         <v>40</v>
       </c>
       <c r="D47">
-        <v>27.7879299274821</v>
+        <v>29.9407753131905</v>
       </c>
       <c r="E47">
-        <v>12.2120700725178</v>
+        <v>-15.1830059519081</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6023,10 +6032,10 @@
         <v>43</v>
       </c>
       <c r="D48">
-        <v>35.892249846392097</v>
+        <v>31.229477322726499</v>
       </c>
       <c r="E48">
-        <v>7.10775015360786</v>
+        <v>0.46321920883848799</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6040,10 +6049,10 @@
         <v>25</v>
       </c>
       <c r="D49">
-        <v>36.399105804072498</v>
+        <v>29.216082170308699</v>
       </c>
       <c r="E49">
-        <v>11.3991058040725</v>
+        <v>5.4073078213821404</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6057,10 +6066,10 @@
         <v>33</v>
       </c>
       <c r="D50">
-        <v>36.772827557642401</v>
+        <v>35.168181599350703</v>
       </c>
       <c r="E50">
-        <v>3.77282755764241</v>
+        <v>9.5648314155457896</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6074,10 +6083,10 @@
         <v>26</v>
       </c>
       <c r="D51">
-        <v>39.267858406592502</v>
+        <v>37.687650699345099</v>
       </c>
       <c r="E51">
-        <v>13.2678584065925</v>
+        <v>4.7501783104002504</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6091,10 +6100,10 @@
         <v>29</v>
       </c>
       <c r="D52">
-        <v>34.000935407786201</v>
+        <v>31.088824122194701</v>
       </c>
       <c r="E52">
-        <v>5.0009354077862502</v>
+        <v>1.8248496956710301</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6108,10 +6117,10 @@
         <v>29</v>
       </c>
       <c r="D53">
-        <v>36.5348078488976</v>
+        <v>30.771657783777901</v>
       </c>
       <c r="E53">
-        <v>7.5348078488976498</v>
+        <v>3.2090998231557899</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6125,10 +6134,10 @@
         <v>54</v>
       </c>
       <c r="D54">
-        <v>50.641506149591997</v>
+        <v>51.434165977789597</v>
       </c>
       <c r="E54">
-        <v>3.3584938504079802</v>
+        <v>-7.9257195972674701</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6142,10 +6151,10 @@
         <v>43</v>
       </c>
       <c r="D55">
-        <v>34.541181921198003</v>
+        <v>35.633390026305499</v>
       </c>
       <c r="E55">
-        <v>8.4588180788019507</v>
+        <v>-2.79533845356009</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6159,10 +6168,10 @@
         <v>51</v>
       </c>
       <c r="D56">
-        <v>45.8215182739902</v>
+        <v>47.7577657376576</v>
       </c>
       <c r="E56">
-        <v>5.1784817260097702</v>
+        <v>-4.4228831706254201</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6176,10 +6185,10 @@
         <v>42</v>
       </c>
       <c r="D57">
-        <v>42.099863350681602</v>
+        <v>42.014473395786801</v>
       </c>
       <c r="E57">
-        <v>9.9863350681658802E-2</v>
+        <v>3.65063598266009</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6193,10 +6202,10 @@
         <v>46</v>
       </c>
       <c r="D58">
-        <v>44.171548696035003</v>
+        <v>45.463936124416399</v>
       </c>
       <c r="E58">
-        <v>1.8284513039649299</v>
+        <v>3.8555922744845601</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6210,10 +6219,10 @@
         <v>54</v>
       </c>
       <c r="D59">
-        <v>51.855151645773503</v>
+        <v>42.255292024751</v>
       </c>
       <c r="E59">
-        <v>2.1448483542264398</v>
+        <v>-3.6033895512207099</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6227,10 +6236,10 @@
         <v>48</v>
       </c>
       <c r="D60">
-        <v>40.928514103108398</v>
+        <v>43.061997955340203</v>
       </c>
       <c r="E60">
-        <v>7.07148589689153</v>
+        <v>-3.8137599526650798</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6244,10 +6253,10 @@
         <v>54</v>
       </c>
       <c r="D61">
-        <v>53.899838644950201</v>
+        <v>52.100591600396903</v>
       </c>
       <c r="E61">
-        <v>0.100161355049785</v>
+        <v>-12.330320590586</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6261,10 +6270,10 @@
         <v>44</v>
       </c>
       <c r="D62">
-        <v>43.384668299450901</v>
+        <v>45.802766529257198</v>
       </c>
       <c r="E62">
-        <v>0.61533170054900599</v>
+        <v>12.055740396794899</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6278,10 +6287,10 @@
         <v>56</v>
       </c>
       <c r="D63">
-        <v>56.100283055795899</v>
+        <v>59.255139387548802</v>
       </c>
       <c r="E63">
-        <v>0.100283055795948</v>
+        <v>0.40871853304422201</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6295,10 +6304,10 @@
         <v>55</v>
       </c>
       <c r="D64">
-        <v>45.517220251676399</v>
+        <v>44.325974296645803</v>
       </c>
       <c r="E64">
-        <v>9.4827797483235905</v>
+        <v>-9.7901364052635795</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6312,10 +6321,10 @@
         <v>56</v>
       </c>
       <c r="D65">
-        <v>38.121241900971597</v>
+        <v>46.631468188432997</v>
       </c>
       <c r="E65">
-        <v>17.8787580990283</v>
+        <v>-12.451641834077201</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6329,10 +6338,10 @@
         <v>54</v>
       </c>
       <c r="D66">
-        <v>54.100014999348403</v>
+        <v>66.124341945859001</v>
       </c>
       <c r="E66">
-        <v>0.10001499934843799</v>
+        <v>-2.16595890789318</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6346,10 +6355,10 @@
         <v>44</v>
       </c>
       <c r="D67">
-        <v>43.899717011046398</v>
+        <v>44.001978034165901</v>
       </c>
       <c r="E67">
-        <v>0.10028298895356599</v>
+        <v>-6.1072529117890504</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6363,10 +6372,10 @@
         <v>46</v>
       </c>
       <c r="D68">
-        <v>47.461893874206098</v>
+        <v>51.441142462891897</v>
       </c>
       <c r="E68">
-        <v>1.4618938742061101</v>
+        <v>-7.5415369459472501</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6380,10 +6389,10 @@
         <v>45</v>
       </c>
       <c r="D69">
-        <v>44.899836121521901</v>
+        <v>45.131561219639003</v>
       </c>
       <c r="E69">
-        <v>0.100163878478056</v>
+        <v>-6.4451178469617698</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6397,10 +6406,10 @@
         <v>51</v>
       </c>
       <c r="D70">
-        <v>45.664306667915596</v>
+        <v>41.754060267874401</v>
       </c>
       <c r="E70">
-        <v>5.3356933320842996</v>
+        <v>-14.9190926712446</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6414,10 +6423,10 @@
         <v>51</v>
       </c>
       <c r="D71">
-        <v>51.1001790300732</v>
+        <v>53.177248498167202</v>
       </c>
       <c r="E71">
-        <v>0.10017903007327</v>
+        <v>15.2213573222023</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6431,10 +6440,10 @@
         <v>49</v>
       </c>
       <c r="D72">
-        <v>42.033484747231803</v>
+        <v>40.313409712177602</v>
       </c>
       <c r="E72">
-        <v>6.96651525276814</v>
+        <v>-4.28807914748554</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6448,10 +6457,10 @@
         <v>59</v>
       </c>
       <c r="D73">
-        <v>52.979465227473099</v>
+        <v>49.437394568283999</v>
       </c>
       <c r="E73">
-        <v>6.0205347725268101</v>
+        <v>-20.40001573488</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6465,10 +6474,10 @@
         <v>39</v>
       </c>
       <c r="D74">
-        <v>38.900275388297999</v>
+        <v>38.2502030602828</v>
       </c>
       <c r="E74">
-        <v>9.9724611701986904E-2</v>
+        <v>3.9214288238769299</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6482,10 +6491,10 @@
         <v>54</v>
       </c>
       <c r="D75">
-        <v>44.667637900748403</v>
+        <v>50.660533383380098</v>
       </c>
       <c r="E75">
-        <v>9.3323620992515703</v>
+        <v>-7.6730559976499899</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6499,10 +6508,10 @@
         <v>34</v>
       </c>
       <c r="D76">
-        <v>32.429158646911297</v>
+        <v>33.106080526896399</v>
       </c>
       <c r="E76">
-        <v>1.57084135308864</v>
+        <v>5.0057380389832096</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6516,10 +6525,10 @@
         <v>27</v>
       </c>
       <c r="D77">
-        <v>26.899515689961</v>
-      </c>
-      <c r="E77">
-        <v>0.100484310038918</v>
+        <v>24.453626360589102</v>
+      </c>
+      <c r="E77" s="4">
+        <v>4.4496782525720304</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6533,10 +6542,10 @@
         <v>17</v>
       </c>
       <c r="D78">
-        <v>36.114611776724999</v>
+        <v>34.6879767974632</v>
       </c>
       <c r="E78">
-        <v>19.114611776724999</v>
+        <v>30.7898971034334</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6550,10 +6559,10 @@
         <v>33</v>
       </c>
       <c r="D79">
-        <v>27.075784156043099</v>
+        <v>26.588181181909601</v>
       </c>
       <c r="E79">
-        <v>5.9242158439568602</v>
+        <v>-1.5771117437567901</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6567,10 +6576,10 @@
         <v>17</v>
       </c>
       <c r="D80">
-        <v>31.0848513919514</v>
+        <v>32.682359114196601</v>
       </c>
       <c r="E80">
-        <v>14.0848513919514</v>
+        <v>21.1055247956328</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6584,10 +6593,10 @@
         <v>37</v>
       </c>
       <c r="D81">
-        <v>38.632936878664701</v>
+        <v>37.558131190232999</v>
       </c>
       <c r="E81">
-        <v>1.63293687866478</v>
+        <v>1.1018096509234701</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6601,10 +6610,10 @@
         <v>26</v>
       </c>
       <c r="D82">
-        <v>40.696595013154599</v>
+        <v>38.509288848816702</v>
       </c>
       <c r="E82">
-        <v>14.696595013154599</v>
+        <v>24.137442188843998</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6618,10 +6627,10 @@
         <v>20</v>
       </c>
       <c r="D83">
-        <v>38.469352092826099</v>
+        <v>46.1646374046299</v>
       </c>
       <c r="E83">
-        <v>18.469352092826099</v>
+        <v>14.378932588657801</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6635,10 +6644,10 @@
         <v>36</v>
       </c>
       <c r="D84">
-        <v>37.376116854446103</v>
+        <v>36.160244681706097</v>
       </c>
       <c r="E84">
-        <v>1.3761168544461599</v>
+        <v>7.6832280872506598</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6652,10 +6661,10 @@
         <v>18</v>
       </c>
       <c r="D85">
-        <v>39.186284558813298</v>
+        <v>36.108411763871999</v>
       </c>
       <c r="E85">
-        <v>21.186284558813298</v>
+        <v>8.8172144904965801</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6669,10 +6678,10 @@
         <v>22</v>
       </c>
       <c r="D86">
-        <v>39.0888283513966</v>
+        <v>36.716638613200701</v>
       </c>
       <c r="E86">
-        <v>17.0888283513966</v>
+        <v>12.393331186656299</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6686,10 +6695,10 @@
         <v>29</v>
       </c>
       <c r="D87">
-        <v>37.548484857039298</v>
+        <v>39.039352856315197</v>
       </c>
       <c r="E87">
-        <v>8.5484848570393197</v>
+        <v>7.8408618956829903</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6703,10 +6712,10 @@
         <v>26</v>
       </c>
       <c r="D88">
-        <v>32.841156365045201</v>
+        <v>35.181789945112698</v>
       </c>
       <c r="E88">
-        <v>6.8411563650452498</v>
+        <v>11.043056252657999</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6720,10 +6729,10 @@
         <v>34</v>
       </c>
       <c r="D89">
-        <v>38.697649878600998</v>
+        <v>36.4754318409653</v>
       </c>
       <c r="E89">
-        <v>4.6976498786010099</v>
+        <v>3.3449030721937598</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6737,10 +6746,10 @@
         <v>16</v>
       </c>
       <c r="D90">
-        <v>35.908904410342203</v>
+        <v>33.821843512517198</v>
       </c>
       <c r="E90">
-        <v>19.908904410342199</v>
+        <v>22.106112259263099</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6754,10 +6763,10 @@
         <v>25</v>
       </c>
       <c r="D91">
-        <v>28.737588932475301</v>
+        <v>27.1890706261613</v>
       </c>
       <c r="E91">
-        <v>3.73758893247531</v>
+        <v>9.5057760020731603</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6771,10 +6780,10 @@
         <v>17</v>
       </c>
       <c r="D92">
-        <v>41.5494130172561</v>
+        <v>43.442655013151899</v>
       </c>
       <c r="E92">
-        <v>24.5494130172561</v>
+        <v>12.8370447637579</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6788,10 +6797,10 @@
         <v>54</v>
       </c>
       <c r="D93">
-        <v>32.992319466073297</v>
+        <v>30.510616795505499</v>
       </c>
       <c r="E93">
-        <v>21.0076805339266</v>
+        <v>-13.54910157129</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6805,10 +6814,10 @@
         <v>47</v>
       </c>
       <c r="D94">
-        <v>42.854863030057103</v>
+        <v>38.6769670990777</v>
       </c>
       <c r="E94">
-        <v>4.1451369699428904</v>
+        <v>-4.4695806199546997</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6822,10 +6831,10 @@
         <v>48</v>
       </c>
       <c r="D95">
-        <v>40.546548316231203</v>
+        <v>42.634502185672702</v>
       </c>
       <c r="E95">
-        <v>7.4534516837686997</v>
+        <v>-6.79098535943454</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6839,10 +6848,10 @@
         <v>20</v>
       </c>
       <c r="D96">
-        <v>36.364936484010698</v>
+        <v>43.275144030487802</v>
       </c>
       <c r="E96">
-        <v>16.364936484010698</v>
+        <v>16.937331736953102</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6856,10 +6865,10 @@
         <v>33</v>
       </c>
       <c r="D97">
-        <v>46.150335478263003</v>
+        <v>51.369831753468603</v>
       </c>
       <c r="E97">
-        <v>13.150335478263001</v>
+        <v>17.597791262280499</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6873,10 +6882,10 @@
         <v>26</v>
       </c>
       <c r="D98">
-        <v>25.322852425029701</v>
+        <v>20.707122561868299</v>
       </c>
       <c r="E98">
-        <v>0.677147574970277</v>
+        <v>16.761978630563501</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6890,10 +6899,10 @@
         <v>50</v>
       </c>
       <c r="D99">
-        <v>39.071471704168502</v>
+        <v>45.734645729068703</v>
       </c>
       <c r="E99">
-        <v>10.9285282958314</v>
+        <v>10.5016210600348</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6907,10 +6916,10 @@
         <v>26</v>
       </c>
       <c r="D100">
-        <v>37.622462844848101</v>
+        <v>36.6928735003141</v>
       </c>
       <c r="E100">
-        <v>11.6224628448481</v>
+        <v>11.874015707950701</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6924,10 +6933,10 @@
         <v>27</v>
       </c>
       <c r="D101">
-        <v>37.826862104934698</v>
+        <v>39.219655296742403</v>
       </c>
       <c r="E101">
-        <v>10.826862104934699</v>
+        <v>9.5627567651437992</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6941,10 +6950,10 @@
         <v>23</v>
       </c>
       <c r="D102">
-        <v>36.362154745594403</v>
+        <v>38.265551221939504</v>
       </c>
       <c r="E102">
-        <v>13.362154745594401</v>
+        <v>9.0630388889924092</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6958,10 +6967,10 @@
         <v>23</v>
       </c>
       <c r="D103">
-        <v>36.711605167762997</v>
+        <v>32.149716921239701</v>
       </c>
       <c r="E103">
-        <v>13.711605167763</v>
+        <v>7.1970293184230503</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6975,10 +6984,10 @@
         <v>44</v>
       </c>
       <c r="D104">
-        <v>39.750242967888497</v>
+        <v>50.106530435544599</v>
       </c>
       <c r="E104">
-        <v>4.2497570321114599</v>
+        <v>-8.23297899317601</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6992,10 +7001,10 @@
         <v>32</v>
       </c>
       <c r="D105">
-        <v>48.072207189195701</v>
+        <v>42.431716047938799</v>
       </c>
       <c r="E105">
-        <v>16.072207189195701</v>
+        <v>3.3666131337578098</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7009,10 +7018,10 @@
         <v>34</v>
       </c>
       <c r="D106">
-        <v>33.605837926034802</v>
+        <v>27.306682267983799</v>
       </c>
       <c r="E106">
-        <v>0.39416207396519098</v>
+        <v>-12.2751211142402</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7026,10 +7035,10 @@
         <v>24</v>
       </c>
       <c r="D107">
-        <v>32.720192035079101</v>
+        <v>27.880768522195002</v>
       </c>
       <c r="E107">
-        <v>8.7201920350790996</v>
+        <v>8.3295493090657899</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7043,10 +7052,10 @@
         <v>17</v>
       </c>
       <c r="D108">
-        <v>38.609762225137899</v>
+        <v>37.520849994424502</v>
       </c>
       <c r="E108">
-        <v>21.609762225137899</v>
+        <v>7.2737829316659797</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7060,10 +7069,10 @@
         <v>24</v>
       </c>
       <c r="D109">
-        <v>26.408579660813601</v>
+        <v>35.382427869003799</v>
       </c>
       <c r="E109">
-        <v>2.40857966081365</v>
+        <v>-0.25433353425597299</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7077,10 +7086,10 @@
         <v>27</v>
       </c>
       <c r="D110">
-        <v>39.007735037365102</v>
+        <v>44.827180034399603</v>
       </c>
       <c r="E110">
-        <v>12.0077350373651</v>
+        <v>13.3627470318796</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7094,10 +7103,10 @@
         <v>26</v>
       </c>
       <c r="D111">
-        <v>43.956310265383898</v>
+        <v>33.978382221365699</v>
       </c>
       <c r="E111">
-        <v>17.956310265383902</v>
+        <v>15.4100325708149</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7111,10 +7120,10 @@
         <v>31</v>
       </c>
       <c r="D112">
-        <v>46.212780580663697</v>
+        <v>43.527217797212202</v>
       </c>
       <c r="E112">
-        <v>15.212780580663701</v>
+        <v>11.0902206449829</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7128,10 +7137,10 @@
         <v>49</v>
       </c>
       <c r="D113">
-        <v>41.865953796069</v>
+        <v>41.987693186910498</v>
       </c>
       <c r="E113">
-        <v>7.1340462039309704</v>
+        <v>-6.5676839552624298</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7145,10 +7154,10 @@
         <v>34</v>
       </c>
       <c r="D114">
-        <v>38.4645287696572</v>
+        <v>35.849507742102901</v>
       </c>
       <c r="E114">
-        <v>4.4645287696572202</v>
+        <v>-4.4127732573008904</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7162,10 +7171,10 @@
         <v>32</v>
       </c>
       <c r="D115">
-        <v>39.1740363264026</v>
+        <v>38.908025469957202</v>
       </c>
       <c r="E115">
-        <v>7.1740363264026099</v>
+        <v>9.2235310011821507</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7179,10 +7188,10 @@
         <v>34</v>
       </c>
       <c r="D116">
-        <v>40.224832126175102</v>
+        <v>44.684065439459303</v>
       </c>
       <c r="E116">
-        <v>6.2248321261751904</v>
+        <v>1.7296402357651499</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7196,10 +7205,10 @@
         <v>30</v>
       </c>
       <c r="D117">
-        <v>40.3339541033138</v>
+        <v>39.570295671241098</v>
       </c>
       <c r="E117">
-        <v>10.3339541033138</v>
+        <v>9.2792505667739604</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7213,10 +7222,10 @@
         <v>29</v>
       </c>
       <c r="D118">
-        <v>39.745369701861499</v>
+        <v>47.322477610990198</v>
       </c>
       <c r="E118">
-        <v>10.745369701861501</v>
+        <v>11.6444415207906</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7230,10 +7239,10 @@
         <v>46</v>
       </c>
       <c r="D119">
-        <v>26.937451755843199</v>
+        <v>36.219868571455798</v>
       </c>
       <c r="E119">
-        <v>19.062548244156702</v>
+        <v>-0.52900101693870705</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7247,10 +7256,10 @@
         <v>34</v>
       </c>
       <c r="D120">
-        <v>48.064344300805402</v>
+        <v>48.382323855131901</v>
       </c>
       <c r="E120">
-        <v>14.0643443008054</v>
+        <v>6.2340362137716596</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7264,10 +7273,10 @@
         <v>20</v>
       </c>
       <c r="D121">
-        <v>37.914047741483103</v>
+        <v>29.861077170684101</v>
       </c>
       <c r="E121">
-        <v>17.914047741483099</v>
+        <v>18.289430615348099</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7281,10 +7290,10 @@
         <v>18</v>
       </c>
       <c r="D122">
-        <v>36.451714695580897</v>
+        <v>36.5256571872862</v>
       </c>
       <c r="E122">
-        <v>18.4517146955809</v>
+        <v>29.9219942017492</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7298,10 +7307,10 @@
         <v>33</v>
       </c>
       <c r="D123">
-        <v>39.328636671610802</v>
+        <v>40.976208036352901</v>
       </c>
       <c r="E123">
-        <v>6.3286366716108802</v>
+        <v>-3.19735007500512</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7315,10 +7324,10 @@
         <v>58</v>
       </c>
       <c r="D124">
-        <v>43.3197762449444</v>
+        <v>33.564657967853002</v>
       </c>
       <c r="E124">
-        <v>14.680223755055501</v>
+        <v>-9.1394860962673405</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7332,10 +7341,10 @@
         <v>59</v>
       </c>
       <c r="D125">
-        <v>39.461882935032001</v>
+        <v>37.682843334165803</v>
       </c>
       <c r="E125">
-        <v>19.538117064967899</v>
+        <v>-15.530545268379999</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7349,10 +7358,10 @@
         <v>45</v>
       </c>
       <c r="D126">
-        <v>45.334642703737003</v>
+        <v>51.078314601706602</v>
       </c>
       <c r="E126">
-        <v>0.33464270373703098</v>
+        <v>-6.7535455027815701</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7366,10 +7375,10 @@
         <v>50</v>
       </c>
       <c r="D127">
-        <v>45.809576890297798</v>
+        <v>38.617671954003598</v>
       </c>
       <c r="E127">
-        <v>4.1904231097021798</v>
+        <v>-5.1548403660301698</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7383,10 +7392,10 @@
         <v>49</v>
       </c>
       <c r="D128">
-        <v>57.735388112369698</v>
+        <v>65.544175244705102</v>
       </c>
       <c r="E128">
-        <v>8.7353881123697406</v>
+        <v>6.3241103629234203</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7400,10 +7409,10 @@
         <v>24</v>
       </c>
       <c r="D129">
-        <v>51.1440037676347</v>
+        <v>48.069771879586803</v>
       </c>
       <c r="E129">
-        <v>27.1440037676347</v>
+        <v>20.980672737769101</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7417,10 +7426,10 @@
         <v>51</v>
       </c>
       <c r="D130">
-        <v>39.1000767453938</v>
+        <v>40.9038774498568</v>
       </c>
       <c r="E130">
-        <v>11.899923254606099</v>
+        <v>12.497745795365899</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7434,10 +7443,10 @@
         <v>35</v>
       </c>
       <c r="D131">
-        <v>42.636565912864</v>
+        <v>40.701301222529402</v>
       </c>
       <c r="E131">
-        <v>7.6365659128640404</v>
+        <v>4.6524424744500896</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7451,10 +7460,10 @@
         <v>52</v>
       </c>
       <c r="D132">
-        <v>35.492044029272002</v>
+        <v>33.799927573418898</v>
       </c>
       <c r="E132">
-        <v>16.507955970727899</v>
+        <v>-8.8081493932750092</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7468,10 +7477,10 @@
         <v>54</v>
       </c>
       <c r="D133">
-        <v>49.0891520890953</v>
+        <v>38.468484711482198</v>
       </c>
       <c r="E133">
-        <v>4.9108479109046597</v>
+        <v>-2.7262205150035901</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7485,10 +7494,10 @@
         <v>43</v>
       </c>
       <c r="D134">
-        <v>46.361262395548003</v>
+        <v>40.100006400568098</v>
       </c>
       <c r="E134">
-        <v>3.3612623955480201</v>
+        <v>-4.6725290353381501</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7502,10 +7511,10 @@
         <v>55</v>
       </c>
       <c r="D135">
-        <v>44.119911060586098</v>
+        <v>49.1387601600225</v>
       </c>
       <c r="E135">
-        <v>10.880088939413801</v>
+        <v>6.0321506036901598</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7519,10 +7528,10 @@
         <v>58</v>
       </c>
       <c r="D136">
-        <v>50.085545835660497</v>
+        <v>54.274425306999298</v>
       </c>
       <c r="E136">
-        <v>7.9144541643394799</v>
+        <v>4.2715304554659701</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7536,10 +7545,10 @@
         <v>50</v>
       </c>
       <c r="D137">
-        <v>42.530619384612898</v>
+        <v>41.846574913058198</v>
       </c>
       <c r="E137">
-        <v>7.4693806153870899</v>
+        <v>-5.8422364342808102</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7553,10 +7562,10 @@
         <v>28</v>
       </c>
       <c r="D138">
-        <v>27.3453524739786</v>
+        <v>25.859993036703202</v>
       </c>
       <c r="E138">
-        <v>0.65464752602135601</v>
+        <v>-4.3221392613941703</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7570,10 +7579,10 @@
         <v>52</v>
       </c>
       <c r="D139">
-        <v>48.698098928612701</v>
+        <v>53.863830820077602</v>
       </c>
       <c r="E139">
-        <v>3.3019010713872201</v>
+        <v>-2.14302454937557</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7587,10 +7596,10 @@
         <v>26</v>
       </c>
       <c r="D140">
-        <v>41.944921697760797</v>
+        <v>37.618733378772603</v>
       </c>
       <c r="E140">
-        <v>15.944921697760799</v>
+        <v>0.75108225712577303</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7604,10 +7613,10 @@
         <v>60</v>
       </c>
       <c r="D141">
-        <v>42.305212992147702</v>
+        <v>45.668474939956802</v>
       </c>
       <c r="E141">
-        <v>17.694787007852199</v>
+        <v>-5.2488171019544003</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7621,10 +7630,10 @@
         <v>58</v>
       </c>
       <c r="D142">
-        <v>50.393439966152002</v>
+        <v>57.153680505875698</v>
       </c>
       <c r="E142">
-        <v>7.6065600338479902</v>
+        <v>9.4845437890954098</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7638,10 +7647,10 @@
         <v>54</v>
       </c>
       <c r="D143">
-        <v>53.224577240702097</v>
+        <v>52.126060386595697</v>
       </c>
       <c r="E143">
-        <v>0.77542275929788196</v>
+        <v>-1.5508923518167499</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7655,10 +7664,10 @@
         <v>21</v>
       </c>
       <c r="D144">
-        <v>43.830946024283499</v>
+        <v>43.039120337885102</v>
       </c>
       <c r="E144">
-        <v>22.830946024283499</v>
+        <v>0.65629795511721001</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7672,10 +7681,10 @@
         <v>53</v>
       </c>
       <c r="D145">
-        <v>41.282272764715998</v>
+        <v>41.126327652105999</v>
       </c>
       <c r="E145">
-        <v>11.717727235283901</v>
+        <v>2.3453819865366898</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7689,10 +7698,10 @@
         <v>50</v>
       </c>
       <c r="D146">
-        <v>41.799278412852502</v>
+        <v>41.756072512285598</v>
       </c>
       <c r="E146">
-        <v>8.2007215871474095</v>
+        <v>22.0147250807943</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7706,10 +7715,10 @@
         <v>28</v>
       </c>
       <c r="D147">
-        <v>35.496207860684898</v>
+        <v>37.070384715380698</v>
       </c>
       <c r="E147">
-        <v>7.4962078606849296</v>
+        <v>14.463907616954399</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7723,10 +7732,10 @@
         <v>60</v>
       </c>
       <c r="D148">
-        <v>37.102687536351802</v>
+        <v>30.960272167689901</v>
       </c>
       <c r="E148">
-        <v>22.897312463648099</v>
+        <v>-15.3331570918397</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7740,10 +7749,10 @@
         <v>28</v>
       </c>
       <c r="D149">
-        <v>36.4855965560022</v>
+        <v>41.760729598279099</v>
       </c>
       <c r="E149">
-        <v>8.4855965560022</v>
+        <v>6.8391448391957796</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7757,10 +7766,10 @@
         <v>54</v>
       </c>
       <c r="D150">
-        <v>53.414694094795102</v>
+        <v>55.600303374261699</v>
       </c>
       <c r="E150">
-        <v>0.58530590520489001</v>
+        <v>-7.0569841875738604</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7774,10 +7783,10 @@
         <v>53</v>
       </c>
       <c r="D151">
-        <v>42.506124102042598</v>
+        <v>32.161620044138303</v>
       </c>
       <c r="E151">
-        <v>10.493875897957301</v>
+        <v>2.6272591521403599</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7791,10 +7800,10 @@
         <v>53</v>
       </c>
       <c r="D152">
-        <v>34.233350896458397</v>
+        <v>31.829203815305601</v>
       </c>
       <c r="E152">
-        <v>18.7666491035415</v>
+        <v>-6.5425641135263604</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7808,10 +7817,10 @@
         <v>43</v>
       </c>
       <c r="D153">
-        <v>37.4367880313184</v>
+        <v>29.942027274854599</v>
       </c>
       <c r="E153">
-        <v>5.56321196868159</v>
+        <v>-3.4432108122736298</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7825,10 +7834,10 @@
         <v>59</v>
       </c>
       <c r="D154">
-        <v>46.367241461185898</v>
+        <v>46.977331114221897</v>
       </c>
       <c r="E154">
-        <v>12.632758538814</v>
+        <v>-9.2317269500347603</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7842,10 +7851,10 @@
         <v>47</v>
       </c>
       <c r="D155">
-        <v>54.673549038333697</v>
+        <v>54.544830002904199</v>
       </c>
       <c r="E155">
-        <v>7.6735490383337401</v>
+        <v>1.5429043739241699</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7859,10 +7868,10 @@
         <v>35</v>
       </c>
       <c r="D156">
-        <v>37.155669667753799</v>
+        <v>35.017926106997301</v>
       </c>
       <c r="E156">
-        <v>2.1556696677537999</v>
+        <v>-2.8012019126312402</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7876,10 +7885,10 @@
         <v>46</v>
       </c>
       <c r="D157">
-        <v>45.883150730561702</v>
+        <v>37.321601931307697</v>
       </c>
       <c r="E157">
-        <v>0.116849269438212</v>
+        <v>1.64183214359008</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7893,10 +7902,10 @@
         <v>52</v>
       </c>
       <c r="D158">
-        <v>57.418475347701403</v>
+        <v>65.217497516712299</v>
       </c>
       <c r="E158">
-        <v>5.41847534770148</v>
+        <v>0.32359814196172398</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7910,10 +7919,10 @@
         <v>42</v>
       </c>
       <c r="D159">
-        <v>52.266870205308699</v>
+        <v>57.109950139614803</v>
       </c>
       <c r="E159">
-        <v>10.266870205308701</v>
+        <v>10.320866247558101</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7927,10 +7936,10 @@
         <v>39</v>
       </c>
       <c r="D160">
-        <v>51.997018417301398</v>
+        <v>49.9844613278145</v>
       </c>
       <c r="E160">
-        <v>12.997018417301399</v>
+        <v>-10.073056296894199</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7944,10 +7953,10 @@
         <v>44</v>
       </c>
       <c r="D161">
-        <v>44.308045735466898</v>
+        <v>38.832614774520003</v>
       </c>
       <c r="E161">
-        <v>0.30804573546692599</v>
+        <v>2.4539090046405301</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7961,10 +7970,10 @@
         <v>53</v>
       </c>
       <c r="D162">
-        <v>52.486483951943796</v>
+        <v>46.707387512751097</v>
       </c>
       <c r="E162">
-        <v>0.51351604805616802</v>
+        <v>15.238080680115999</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -7978,10 +7987,10 @@
         <v>53</v>
       </c>
       <c r="D163">
-        <v>54.844813889198399</v>
+        <v>56.385740982943403</v>
       </c>
       <c r="E163">
-        <v>1.84481388919844</v>
+        <v>-13.601594582351099</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7995,10 +8004,10 @@
         <v>34</v>
       </c>
       <c r="D164">
-        <v>52.214365503752802</v>
+        <v>68.177171360494199</v>
       </c>
       <c r="E164">
-        <v>18.214365503752799</v>
+        <v>10.6665566133375</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8012,10 +8021,10 @@
         <v>52</v>
       </c>
       <c r="D165">
-        <v>35.058803568911003</v>
+        <v>33.202179770785101</v>
       </c>
       <c r="E165">
-        <v>16.941196431088901</v>
+        <v>-8.6821511934090198E-2</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8029,10 +8038,10 @@
         <v>55</v>
       </c>
       <c r="D166">
-        <v>35.938115788557397</v>
+        <v>27.228419955397101</v>
       </c>
       <c r="E166">
-        <v>19.0618842114425</v>
+        <v>-0.64267623116005201</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8046,10 +8055,10 @@
         <v>28</v>
       </c>
       <c r="D167">
-        <v>45.869056664677899</v>
+        <v>53.9542789867726</v>
       </c>
       <c r="E167">
-        <v>17.869056664677899</v>
+        <v>11.3602594163678</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8063,10 +8072,10 @@
         <v>45</v>
       </c>
       <c r="D168">
-        <v>44.659612292983503</v>
+        <v>40.341120125721098</v>
       </c>
       <c r="E168">
-        <v>0.34038770701646798</v>
+        <v>12.123667049830299</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8080,10 +8089,10 @@
         <v>46</v>
       </c>
       <c r="D169">
-        <v>41.486200443827101</v>
+        <v>46.803738332670001</v>
       </c>
       <c r="E169">
-        <v>4.5137995561728204</v>
+        <v>18.671589562352601</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8097,10 +8106,10 @@
         <v>55</v>
       </c>
       <c r="D170">
-        <v>54.352520427556698</v>
+        <v>56.641643886983402</v>
       </c>
       <c r="E170">
-        <v>0.64747957244321697</v>
+        <v>-5.2145677958866798</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8114,10 +8123,10 @@
         <v>41</v>
       </c>
       <c r="D171">
-        <v>34.7606983922078</v>
+        <v>35.126213564132101</v>
       </c>
       <c r="E171">
-        <v>6.2393016077921901</v>
+        <v>7.0165939416493703</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8131,10 +8140,10 @@
         <v>45</v>
       </c>
       <c r="D172">
-        <v>44.485459198698202</v>
+        <v>40.562449066568099</v>
       </c>
       <c r="E172">
-        <v>0.51454080130173396</v>
+        <v>3.96567983792389</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8148,10 +8157,10 @@
         <v>42</v>
       </c>
       <c r="D173">
-        <v>42.764788355397201</v>
+        <v>30.522432660589001</v>
       </c>
       <c r="E173">
-        <v>0.76478835539725698</v>
+        <v>2.6429811818782798</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8165,10 +8174,10 @@
         <v>34</v>
       </c>
       <c r="D174">
-        <v>34.187426527661799</v>
+        <v>28.4910914119083</v>
       </c>
       <c r="E174">
-        <v>0.187426527661813</v>
+        <v>7.7929654887514301</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8182,10 +8191,10 @@
         <v>48</v>
       </c>
       <c r="D175">
-        <v>35.113289115113602</v>
+        <v>26.856707002731198</v>
       </c>
       <c r="E175">
-        <v>12.8867108848863</v>
+        <v>-19.526122135978</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8199,10 +8208,10 @@
         <v>50</v>
       </c>
       <c r="D176">
-        <v>45.2595589825738</v>
+        <v>35.913481874332703</v>
       </c>
       <c r="E176">
-        <v>4.7404410174261704</v>
+        <v>4.1608377028338799</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8216,10 +8225,10 @@
         <v>36</v>
       </c>
       <c r="D177">
-        <v>50.822037118659203</v>
+        <v>49.873644334599597</v>
       </c>
       <c r="E177">
-        <v>14.8220371186592</v>
+        <v>8.4526280968683203</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8233,10 +8242,10 @@
         <v>49</v>
       </c>
       <c r="D178">
-        <v>48.728729976971003</v>
+        <v>48.531424626844696</v>
       </c>
       <c r="E178">
-        <v>0.27127002302890402</v>
+        <v>-0.475036619129731</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8250,10 +8259,10 @@
         <v>53</v>
       </c>
       <c r="D179">
-        <v>44.775482614498699</v>
+        <v>43.709941163363702</v>
       </c>
       <c r="E179">
-        <v>8.2245173855012297</v>
+        <v>-5.5415302566624902</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8267,10 +8276,10 @@
         <v>51</v>
       </c>
       <c r="D180">
-        <v>40.003705887049598</v>
+        <v>23.991686039250801</v>
       </c>
       <c r="E180">
-        <v>10.9962941129503</v>
+        <v>-0.66792906667808405</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8284,10 +8293,10 @@
         <v>46</v>
       </c>
       <c r="D181">
-        <v>42.479559413844697</v>
+        <v>39.559371748472103</v>
       </c>
       <c r="E181">
-        <v>3.5204405861552299</v>
+        <v>-5.7968973045812797</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8301,10 +8310,10 @@
         <v>55</v>
       </c>
       <c r="D182">
-        <v>52.396807008219596</v>
+        <v>63.294002073540597</v>
       </c>
       <c r="E182">
-        <v>2.6031929917803098</v>
+        <v>-15.637360519805201</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8318,10 +8327,10 @@
         <v>47</v>
       </c>
       <c r="D183">
-        <v>40.5740675289153</v>
+        <v>46.447317274431903</v>
       </c>
       <c r="E183">
-        <v>6.4259324710846597</v>
+        <v>-11.805903242207799</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8335,10 +8344,10 @@
         <v>52</v>
       </c>
       <c r="D184">
-        <v>49.762904985637</v>
+        <v>57.323257595045398</v>
       </c>
       <c r="E184">
-        <v>2.23709501436291</v>
+        <v>0.51650861183276198</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8352,10 +8361,10 @@
         <v>39</v>
       </c>
       <c r="D185">
-        <v>45.813875606728502</v>
+        <v>49.982348232181103</v>
       </c>
       <c r="E185">
-        <v>6.8138756067285797</v>
+        <v>-1.99019756474065</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8369,10 +8378,10 @@
         <v>59</v>
       </c>
       <c r="D186">
-        <v>53.106024902402503</v>
+        <v>55.896592718591997</v>
       </c>
       <c r="E186">
-        <v>5.8939750975974503</v>
+        <v>9.3005934962305101</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8386,10 +8395,10 @@
         <v>49</v>
       </c>
       <c r="D187">
-        <v>55.495329436223003</v>
+        <v>55.602353932023199</v>
       </c>
       <c r="E187">
-        <v>6.4953294362230496</v>
+        <v>-9.1124708189614196</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8403,10 +8412,10 @@
         <v>52</v>
       </c>
       <c r="D188">
-        <v>51.801695129492302</v>
+        <v>54.784610177555699</v>
       </c>
       <c r="E188">
-        <v>0.19830487050766199</v>
+        <v>1.5585622901790399</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8420,10 +8429,10 @@
         <v>41</v>
       </c>
       <c r="D189">
-        <v>52.8662147089616</v>
+        <v>55.731596008104503</v>
       </c>
       <c r="E189">
-        <v>11.8662147089616</v>
+        <v>-6.3394826997406897</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8437,10 +8446,10 @@
         <v>45</v>
       </c>
       <c r="D190">
-        <v>53.8661965746576</v>
+        <v>56.2974542095102</v>
       </c>
       <c r="E190">
-        <v>8.8661965746576499</v>
+        <v>-7.6464748701648704</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8454,10 +8463,10 @@
         <v>61</v>
       </c>
       <c r="D191">
-        <v>44.549384159375897</v>
+        <v>52.443088255354198</v>
       </c>
       <c r="E191">
-        <v>16.450615840624</v>
+        <v>-7.7996936103173198</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8471,10 +8480,10 @@
         <v>55</v>
       </c>
       <c r="D192">
-        <v>47.155023386862297</v>
+        <v>44.171794240058702</v>
       </c>
       <c r="E192">
-        <v>7.8449766131376801</v>
+        <v>-0.162984122908468</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8488,10 +8497,10 @@
         <v>61</v>
       </c>
       <c r="D193">
-        <v>39.819318933911298</v>
+        <v>42.683858304298496</v>
       </c>
       <c r="E193">
-        <v>21.180681066088599</v>
+        <v>5.0825203412631401</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8505,10 +8514,10 @@
         <v>56</v>
       </c>
       <c r="D194">
-        <v>47.126207003095899</v>
+        <v>38.963578027048897</v>
       </c>
       <c r="E194">
-        <v>8.8737929969041005</v>
+        <v>-9.7266780688147794</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8522,10 +8531,10 @@
         <v>48</v>
       </c>
       <c r="D195">
-        <v>41.003430152633001</v>
+        <v>43.720742507527397</v>
       </c>
       <c r="E195">
-        <v>6.9965698473669198</v>
+        <v>-16.0812623813603</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8539,10 +8548,10 @@
         <v>48</v>
       </c>
       <c r="D196">
-        <v>40.915370861385597</v>
+        <v>32.525714241756297</v>
       </c>
       <c r="E196">
-        <v>7.0846291386143596</v>
+        <v>-8.4565492026295797</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8556,10 +8565,10 @@
         <v>62</v>
       </c>
       <c r="D197">
-        <v>52.923976207814199</v>
+        <v>53.271614324390399</v>
       </c>
       <c r="E197">
-        <v>9.0760237921857208</v>
+        <v>-4.2859005183277601</v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -8573,10 +8582,10 @@
         <v>55</v>
       </c>
       <c r="D198">
-        <v>49.840491933804699</v>
+        <v>51.191504394853297</v>
       </c>
       <c r="E198">
-        <v>5.1595080661952499</v>
+        <v>-3.8084956051466099</v>
       </c>
     </row>
     <row r="199" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Comments code, finishes Readme. Adds some new data.
</commit_message>
<xml_diff>
--- a/PredictedAges.xlsx
+++ b/PredictedAges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\Graduate School\Summer 2019\Chen Research\BrainAgePredictor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wurster.18\Documents\GitHub\BrainAgePredictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C05589-096F-4945-A20E-FEC4129C4DBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8D3085-C564-4302-A3AD-2FB88D3A7BFA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7785" xr2:uid="{3ABF37D0-9CE1-4972-898F-CECF5263D171}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3ABF37D0-9CE1-4972-898F-CECF5263D171}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>